<commit_message>
letras pablo con etiqueta
</commit_message>
<xml_diff>
--- a/Codigo/LETRAS/O.xlsx
+++ b/Codigo/LETRAS/O.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2N QUATRIMESTRE\RLP\Projecte\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C466A8FA-707B-4CBF-9BB0-10D5D18E2139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -148,8 +154,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,11 +218,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -258,7 +272,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,9 +304,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,6 +356,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,14 +549,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AM39" workbookViewId="0">
+      <selection activeCell="AU57" sqref="AU57"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,7 +689,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -768,10 +820,10 @@
         <v>66</v>
       </c>
       <c r="AR2">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -902,10 +954,10 @@
         <v>110</v>
       </c>
       <c r="AR3">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1036,10 +1088,10 @@
         <v>108</v>
       </c>
       <c r="AR4">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1170,10 +1222,10 @@
         <v>117</v>
       </c>
       <c r="AR5">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1304,10 +1356,10 @@
         <v>123</v>
       </c>
       <c r="AR6">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1438,10 +1490,10 @@
         <v>122</v>
       </c>
       <c r="AR7">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1572,10 +1624,10 @@
         <v>126</v>
       </c>
       <c r="AR8">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1706,10 +1758,10 @@
         <v>128</v>
       </c>
       <c r="AR9">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1840,10 +1892,10 @@
         <v>136</v>
       </c>
       <c r="AR10">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1974,10 +2026,10 @@
         <v>152</v>
       </c>
       <c r="AR11">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2108,10 +2160,10 @@
         <v>149</v>
       </c>
       <c r="AR12">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2242,10 +2294,10 @@
         <v>145</v>
       </c>
       <c r="AR13">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2376,10 +2428,10 @@
         <v>139</v>
       </c>
       <c r="AR14">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2510,10 +2562,10 @@
         <v>140</v>
       </c>
       <c r="AR15">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2644,10 +2696,10 @@
         <v>142</v>
       </c>
       <c r="AR16">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:44">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2778,10 +2830,10 @@
         <v>144</v>
       </c>
       <c r="AR17">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:44">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2912,10 +2964,10 @@
         <v>145</v>
       </c>
       <c r="AR18">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:44">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3046,10 +3098,10 @@
         <v>149</v>
       </c>
       <c r="AR19">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:44">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3180,10 +3232,10 @@
         <v>154</v>
       </c>
       <c r="AR20">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:44">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3314,10 +3366,10 @@
         <v>153</v>
       </c>
       <c r="AR21">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:44">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3448,10 +3500,10 @@
         <v>145</v>
       </c>
       <c r="AR22">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:44">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3582,10 +3634,10 @@
         <v>120</v>
       </c>
       <c r="AR23">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:44">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3716,10 +3768,10 @@
         <v>123</v>
       </c>
       <c r="AR24">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:44">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3850,10 +3902,10 @@
         <v>132</v>
       </c>
       <c r="AR25">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:44">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3984,10 +4036,10 @@
         <v>133</v>
       </c>
       <c r="AR26">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:44">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -4118,10 +4170,10 @@
         <v>124</v>
       </c>
       <c r="AR27">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:44">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -4252,10 +4304,10 @@
         <v>138</v>
       </c>
       <c r="AR28">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:44">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -4386,10 +4438,10 @@
         <v>143</v>
       </c>
       <c r="AR29">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:44">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -4520,10 +4572,10 @@
         <v>68</v>
       </c>
       <c r="AR30">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:44">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4654,10 +4706,10 @@
         <v>124</v>
       </c>
       <c r="AR31">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:44">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -4788,10 +4840,10 @@
         <v>127</v>
       </c>
       <c r="AR32">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:44">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -4922,10 +4974,10 @@
         <v>126</v>
       </c>
       <c r="AR33">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:44">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -5056,10 +5108,10 @@
         <v>117</v>
       </c>
       <c r="AR34">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:44">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -5190,10 +5242,10 @@
         <v>384</v>
       </c>
       <c r="AR35">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:44">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -5324,10 +5376,10 @@
         <v>122</v>
       </c>
       <c r="AR36">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:44">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -5458,10 +5510,10 @@
         <v>121</v>
       </c>
       <c r="AR37">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:44">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -5592,10 +5644,10 @@
         <v>137</v>
       </c>
       <c r="AR38">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:44">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -5726,10 +5778,10 @@
         <v>135</v>
       </c>
       <c r="AR39">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:44">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -5860,10 +5912,10 @@
         <v>143</v>
       </c>
       <c r="AR40">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:44">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -5994,10 +6046,10 @@
         <v>143</v>
       </c>
       <c r="AR41">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:44">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -6128,10 +6180,10 @@
         <v>144</v>
       </c>
       <c r="AR42">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:44">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -6262,10 +6314,10 @@
         <v>144</v>
       </c>
       <c r="AR43">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:44">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -6396,10 +6448,10 @@
         <v>146</v>
       </c>
       <c r="AR44">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:44">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -6530,10 +6582,10 @@
         <v>137</v>
       </c>
       <c r="AR45">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:44">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -6664,10 +6716,10 @@
         <v>130</v>
       </c>
       <c r="AR46">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:44">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -6798,10 +6850,10 @@
         <v>136</v>
       </c>
       <c r="AR47">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:44">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -6932,10 +6984,10 @@
         <v>136</v>
       </c>
       <c r="AR48">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:44">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -7066,10 +7118,10 @@
         <v>144</v>
       </c>
       <c r="AR49">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:44">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -7200,10 +7252,10 @@
         <v>152</v>
       </c>
       <c r="AR50">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:44">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -7334,7 +7386,7 @@
         <v>147</v>
       </c>
       <c r="AR51">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>